<commit_message>
add web ui robot
</commit_message>
<xml_diff>
--- a/test_cases/web_test_cases.xlsx
+++ b/test_cases/web_test_cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" activeTab="2"/>
+    <workbookView windowWidth="28125" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>Case ID</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Descriptions</t>
   </si>
   <si>
     <t>Run</t>
   </si>
   <si>
+    <t>Tags</t>
+  </si>
+  <si>
     <t>TC001</t>
   </si>
   <si>
@@ -36,6 +42,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>tag1</t>
   </si>
   <si>
     <t>TC002</t>
@@ -136,12 +145,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,7 +184,58 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,44 +249,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -260,57 +282,50 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,187 +340,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF212121"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,6 +618,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -611,30 +652,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
@@ -655,131 +676,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -791,6 +812,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1139,19 +1167,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="8.28703703703704" customWidth="1"/>
-    <col min="2" max="2" width="33.712962962963" customWidth="1"/>
+    <col min="1" max="1" width="8.28571428571429" customWidth="1"/>
+    <col min="2" max="2" width="6.71428571428571" customWidth="1"/>
+    <col min="3" max="3" width="33.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="5.57142857142857" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:3">
+    <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,33 +1191,46 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" spans="1:3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,15 +1244,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="7.86111111111111" customWidth="1"/>
-    <col min="3" max="3" width="11.712962962963" customWidth="1"/>
-    <col min="4" max="4" width="19.4259259259259" customWidth="1"/>
+    <col min="2" max="2" width="7.85714285714286" customWidth="1"/>
+    <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="19.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1218,50 +1261,50 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1275,110 +1318,110 @@
   <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="24.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="15.287037037037" customWidth="1"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="24.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="17.4259259259259" customWidth="1"/>
+    <col min="5" max="5" width="17.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1404,54 +1447,54 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="14.8611111111111" customWidth="1"/>
-    <col min="3" max="3" width="13.1388888888889" customWidth="1"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1469,11 +1512,11 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="8.28703703703704" customWidth="1"/>
+    <col min="1" max="2" width="8.28571428571429" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.712962962963" customWidth="1"/>
+    <col min="4" max="4" width="23.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:4">
@@ -1481,97 +1524,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reports dir and add modify cookie
</commit_message>
<xml_diff>
--- a/test_cases/web_test_cases.xlsx
+++ b/test_cases/web_test_cases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>Suite</t>
   </si>
@@ -101,6 +101,12 @@
     <t>url</t>
   </si>
   <si>
+    <t>modify_server_side_cookie</t>
+  </si>
+  <si>
+    <t>url,intercept_url_pattern,cookie</t>
+  </si>
+  <si>
     <t>SearchBox</t>
   </si>
   <si>
@@ -155,13 +161,31 @@
     <t>${url}</t>
   </si>
   <si>
+    <t>intercept_url_pattern</t>
+  </si>
+  <si>
+    <t>cookie</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>{"name":"H_PS_PSSID","value":"111222333"}</t>
+  </si>
+  <si>
     <t>TC001功能测试</t>
   </si>
   <si>
     <t>百度搜索</t>
   </si>
   <si>
+    <t>{"name":"H_PS_PSSID","value":"444555666"}</t>
+  </si>
+  <si>
     <t>TC001性能测试</t>
+  </si>
+  <si>
+    <t>{"name":"H_PS_PSSID","value":"777888999"}</t>
   </si>
   <si>
     <t>TC002自动化测试</t>
@@ -223,7 +247,7 @@
   "no-sandbox": true,
   "disable-dev-shm-usage": true,
   "disable-gpu": true,
-  "remote-debugging-port": 9222,
+  "remote-debugging-port": "9222",
   "headless": true
 }</t>
   </si>
@@ -242,7 +266,7 @@
   "no-sandbox": true,
   "disable-dev-shm-usage": true,
   "disable-gpu": true,
-  "remote-debugging-port": 9222
+  "remote-debugging-port": "9222"
 }</t>
   </si>
   <si>
@@ -252,7 +276,7 @@
     <t>Variable Value</t>
   </si>
   <si>
-    <t>http://www.baidu.com</t>
+    <t>https://www.baidu.com/</t>
   </si>
   <si>
     <t>Action Name</t>
@@ -344,9 +368,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -389,7 +413,98 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,8 +518,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,68 +540,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -486,43 +547,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
@@ -550,12 +574,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -568,13 +694,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,151 +754,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,36 +779,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -824,15 +818,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -851,6 +836,45 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -859,7 +883,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
@@ -880,127 +904,127 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1536,19 +1560,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="24.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="15.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="17.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="30.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="9.28571428571429" style="12" customWidth="1"/>
     <col min="7" max="7" width="11.2857142857143" style="12" customWidth="1"/>
     <col min="8" max="8" width="9" style="5"/>
@@ -1611,20 +1635,18 @@
       <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>8</v>
-      </c>
+      <c r="F3" s="8"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="13">
+        <v>1</v>
+      </c>
       <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1637,21 +1659,19 @@
         <v>17</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="9"/>
       <c r="F4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1663,21 +1683,27 @@
       <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="D5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
       <c r="I5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:9">
+    <row r="6" ht="15.75" customHeight="1" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
@@ -1688,7 +1714,9 @@
       <c r="D6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -1696,9 +1724,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" ht="15.75" spans="1:9">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C4 C5 C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C4 C5 C6 C7">
       <formula1>Locators!$B$2:$B$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -1732,10 +1779,10 @@
         <v>18</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:4">
@@ -1743,13 +1790,13 @@
         <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:4">
@@ -1757,13 +1804,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1775,19 +1822,19 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="8.28571428571429" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="20.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="10.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="23.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="42.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
@@ -1795,16 +1842,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:5">
@@ -1819,7 +1866,7 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:5">
@@ -1830,11 +1877,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="11" t="s">
-        <v>44</v>
+      <c r="E3" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:5">
@@ -1845,11 +1892,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:5">
@@ -1857,14 +1906,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
-        <v>43</v>
+      <c r="E5" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:5">
@@ -1872,14 +1921,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:5">
@@ -1890,56 +1939,150 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:5">
       <c r="A8" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" spans="1:5">
+      <c r="D9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>48</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" spans="1:5">
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" spans="1:5">
+      <c r="A16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +2097,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1973,89 +2116,89 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="120" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="105" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2074,7 +2217,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2088,41 +2231,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
-    <hyperlink ref="C3" r:id="rId1" display="http://www.baidu.com" tooltip="http://www.baidu.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.baidu.com/" tooltip="https://www.baidu.com/"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.baidu.com/" tooltip="https://www.baidu.com/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2148,35 +2291,35 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="60" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>